<commit_message>
Sprint 4 daily stand up, day 1
</commit_message>
<xml_diff>
--- a/Documentation and designs/Sprint_info/Sprint4.xlsx
+++ b/Documentation and designs/Sprint_info/Sprint4.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nevidjen\Documents\GitHub\MasterAudioTechnologyFunctions\Documentation and designs\Sprint_info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT\MasterAudioTechnologyFunctions\Documentation and designs\Sprint_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="2" r:id="rId1"/>
@@ -596,6 +596,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -627,7 +628,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sr-Latn-RS"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -999,7 +1000,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="sr-Latn-RS"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1036,7 +1037,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sr-Latn-RS"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="308624616"/>
@@ -1092,6 +1093,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1116,7 +1118,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="sr-Latn-RS"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1147,7 +1149,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sr-Latn-RS"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="308619040"/>
@@ -1198,7 +1200,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sr-Latn-RS"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1246,7 +1248,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="sr-Latn-RS"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1912,23 +1914,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1964,23 +1949,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2217,13 +2185,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
     <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3002,7 +2970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added few changes in sprint info
</commit_message>
<xml_diff>
--- a/Documentation and designs/Sprint_info/Sprint4.xlsx
+++ b/Documentation and designs/Sprint_info/Sprint4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -911,7 +911,7 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2217,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2406,7 +2406,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
@@ -2423,10 +2423,12 @@
       <c r="Q7" s="19"/>
       <c r="R7" s="19"/>
       <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
+      <c r="T7" s="19">
+        <v>2</v>
+      </c>
       <c r="U7" s="19">
         <f t="shared" ref="U7:U15" si="0">E7-SUM(G7:T7)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2476,7 +2478,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
@@ -2491,10 +2493,12 @@
       <c r="Q9" s="19"/>
       <c r="R9" s="19"/>
       <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
+      <c r="T9" s="19">
+        <v>1</v>
+      </c>
       <c r="U9" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2510,7 +2514,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -2525,10 +2529,12 @@
       <c r="Q10" s="19"/>
       <c r="R10" s="19"/>
       <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
+      <c r="T10" s="19">
+        <v>2</v>
+      </c>
       <c r="U10" s="19">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2582,7 +2588,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -2597,10 +2603,12 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
+      <c r="T12" s="2">
+        <v>3</v>
+      </c>
       <c r="U12" s="19">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -2641,12 +2649,14 @@
       <c r="C14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E14" s="2">
         <v>8</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -2661,10 +2671,12 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
+      <c r="T14" s="2">
+        <v>8</v>
+      </c>
       <c r="U14" s="19">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -2673,12 +2685,14 @@
       <c r="C15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E15" s="2">
         <v>1</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -2768,11 +2782,11 @@
       </c>
       <c r="T16" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U16" s="2">
         <f t="shared" ref="U16" si="2">E16-SUM(G16:T16)</f>
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -2911,7 +2925,7 @@
       </c>
       <c r="T18" s="2">
         <f>S18-SUM(T5:T15)</f>
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="U18" s="10"/>
     </row>
@@ -3006,7 +3020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>